<commit_message>
Intermediate check-in to update js-xlsx library and update to macGenFormDef.sh to work on Windows
</commit_message>
<xml_diff>
--- a/app/tables/visit/forms/visit/visit.xlsx
+++ b/app/tables/visit/forms/visit/visit.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="940" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="101">
   <si>
     <t>setting_name</t>
   </si>
@@ -168,9 +168,6 @@
     <t>decimal</t>
   </si>
   <si>
-    <t>What is the height of the plant in feet?</t>
-  </si>
-  <si>
     <t>select_linked_plot</t>
   </si>
   <si>
@@ -322,13 +319,19 @@
   </si>
   <si>
     <t>table_id</t>
+  </si>
+  <si>
+    <t>disableSwipeNavigation</t>
+  </si>
+  <si>
+    <t>What is the height of the plant in inches?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -365,6 +368,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -488,7 +497,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -520,6 +529,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -948,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -992,10 +1004,10 @@
         <v>15</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>24</v>
@@ -1017,24 +1029,24 @@
         <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:7">
       <c r="D6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
         <v>42</v>
@@ -1046,98 +1058,98 @@
     <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A7" s="12"/>
       <c r="B7" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="12"/>
       <c r="B8" s="4"/>
       <c r="D8" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A10" s="12"/>
       <c r="B10" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A11" s="12"/>
       <c r="B11" s="4"/>
       <c r="D11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A12" s="12"/>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A13" s="12"/>
       <c r="B13" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A14" s="12"/>
       <c r="B14" s="4"/>
       <c r="D14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A15" s="12"/>
       <c r="B15" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A16" s="12"/>
       <c r="B16" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="D17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" t="s">
         <v>54</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -1158,107 +1170,107 @@
     <row r="20" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A20" s="12"/>
       <c r="B20" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A21" s="12"/>
       <c r="B21" s="4"/>
       <c r="D21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A22" s="12"/>
       <c r="B22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A23" s="12"/>
       <c r="B23" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="12"/>
       <c r="B24" s="4"/>
       <c r="D24" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A25" s="12"/>
       <c r="B25" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A26" s="12"/>
       <c r="B26" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A27" s="12"/>
       <c r="B27" s="4"/>
       <c r="D27" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A28" s="12"/>
       <c r="B28" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A29" s="12"/>
       <c r="B29" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A30" s="12"/>
       <c r="B30" s="4"/>
       <c r="D30" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A31" s="12"/>
       <c r="B31" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
       <c r="A32" s="12"/>
       <c r="B32" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="4:7">
@@ -1266,13 +1278,13 @@
         <v>15</v>
       </c>
       <c r="E33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F33" t="s">
         <v>33</v>
       </c>
       <c r="G33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="4:7">
@@ -1329,38 +1341,38 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1370,47 +1382,47 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1423,11 +1435,11 @@
         <v>41</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1439,7 +1451,7 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1451,7 +1463,7 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1463,7 +1475,7 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1516,12 +1528,12 @@
         <v>21</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>22</v>
@@ -1531,13 +1543,13 @@
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1553,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1603,10 +1615,18 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30">
+      <c r="A6" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>